<commit_message>
added new method for simplified gathering of data for a whole year
</commit_message>
<xml_diff>
--- a/inst/extdata/_Rotenfels_Gesamt_Template.xlsx
+++ b/inst/extdata/_Rotenfels_Gesamt_Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
   <si>
     <t>Datum</t>
   </si>
@@ -207,6 +207,15 @@
   </si>
   <si>
     <t>Pluvio_mm</t>
+  </si>
+  <si>
+    <t>Pluvio_mm_SUM</t>
+  </si>
+  <si>
+    <t>Niederschlag.Casella</t>
+  </si>
+  <si>
+    <t>Niederschlag.Casella_SUM</t>
   </si>
 </sst>
 </file>
@@ -280,7 +289,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -683,8 +692,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141245824"/>
-        <c:axId val="141251712"/>
+        <c:axId val="264634368"/>
+        <c:axId val="264635904"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -737,11 +746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141268096"/>
-        <c:axId val="141253632"/>
+        <c:axId val="264640000"/>
+        <c:axId val="264637824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141245824"/>
+        <c:axId val="264634368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43102"/>
@@ -753,13 +762,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141251712"/>
+        <c:crossAx val="264635904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="91"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141251712"/>
+        <c:axId val="264635904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -790,12 +799,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141245824"/>
+        <c:crossAx val="264634368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141253632"/>
+        <c:axId val="264637824"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="25"/>
@@ -824,12 +833,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141268096"/>
+        <c:crossAx val="264640000"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141268096"/>
+        <c:axId val="264640000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +848,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141253632"/>
+        <c:crossAx val="264637824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -858,7 +867,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -885,7 +894,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1262,8 +1270,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133112960"/>
-        <c:axId val="133114496"/>
+        <c:axId val="265243264"/>
+        <c:axId val="265257344"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1316,11 +1324,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133130880"/>
-        <c:axId val="133128960"/>
+        <c:axId val="265265536"/>
+        <c:axId val="265259264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133112960"/>
+        <c:axId val="265243264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43102"/>
@@ -1332,13 +1340,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133114496"/>
+        <c:crossAx val="265257344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="91"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133114496"/>
+        <c:axId val="265257344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1361,19 +1369,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133112960"/>
+        <c:crossAx val="265243264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133128960"/>
+        <c:axId val="265259264"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="25"/>
@@ -1396,19 +1403,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133130880"/>
+        <c:crossAx val="265265536"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133130880"/>
+        <c:axId val="265265536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1418,14 +1424,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133128960"/>
+        <c:crossAx val="265259264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1438,7 +1443,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1465,7 +1470,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1842,8 +1846,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133181440"/>
-        <c:axId val="133182976"/>
+        <c:axId val="291182080"/>
+        <c:axId val="291183616"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1896,11 +1900,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133191168"/>
-        <c:axId val="133184896"/>
+        <c:axId val="300289024"/>
+        <c:axId val="300287104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133181440"/>
+        <c:axId val="291182080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43102"/>
@@ -1912,13 +1916,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133182976"/>
+        <c:crossAx val="291183616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="91"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133182976"/>
+        <c:axId val="291183616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1943,20 +1947,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133181440"/>
+        <c:crossAx val="291182080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133184896"/>
+        <c:axId val="300287104"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="25"/>
@@ -1979,19 +1982,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133191168"/>
+        <c:crossAx val="300289024"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133191168"/>
+        <c:axId val="300289024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2001,14 +2003,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133184896"/>
+        <c:crossAx val="300287104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2021,7 +2022,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2048,7 +2049,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2185,11 +2185,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141310976"/>
-        <c:axId val="141329152"/>
+        <c:axId val="300327680"/>
+        <c:axId val="300329216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141310976"/>
+        <c:axId val="300327680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="43102"/>
@@ -2201,13 +2201,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141329152"/>
+        <c:crossAx val="300329216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="91"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141329152"/>
+        <c:axId val="300329216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2230,21 +2230,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141310976"/>
+        <c:crossAx val="300327680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2257,7 +2255,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2289,7 +2287,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2354,8 +2351,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141348224"/>
-        <c:axId val="141579392"/>
+        <c:axId val="326243456"/>
+        <c:axId val="326244992"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2418,11 +2415,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141583488"/>
-        <c:axId val="141581312"/>
+        <c:axId val="326249088"/>
+        <c:axId val="326247168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141348224"/>
+        <c:axId val="326243456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42735"/>
@@ -2434,13 +2431,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141579392"/>
+        <c:crossAx val="326244992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="91"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141579392"/>
+        <c:axId val="326244992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -2465,19 +2462,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141348224"/>
+        <c:crossAx val="326243456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141581312"/>
+        <c:axId val="326247168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2501,20 +2497,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141583488"/>
+        <c:crossAx val="326249088"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141583488"/>
+        <c:axId val="326249088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2524,14 +2519,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141581312"/>
+        <c:crossAx val="326247168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2544,7 +2538,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2587,7 +2581,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>Freiland!$D$1</c:f>
@@ -2617,6 +2611,86 @@
           <c:yVal>
             <c:numRef>
               <c:f>Freiland!$D$3:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Freiland!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pluvio_mm_SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Freiland!$A$3:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Freiland!$J$3:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Freiland!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Niederschlag.Casella_SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700"/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Freiland!$A$3:$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Freiland!$L$3:$L$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2633,15 +2707,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="142266368"/>
-        <c:axId val="142267904"/>
+        <c:axId val="326301184"/>
+        <c:axId val="326302720"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Freiland!$C$1</c:f>
@@ -2689,7 +2763,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>Freiland!$I$1</c:f>
@@ -2735,11 +2809,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141755904"/>
-        <c:axId val="142269824"/>
+        <c:axId val="33819648"/>
+        <c:axId val="33817728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="142266368"/>
+        <c:axId val="326301184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42735"/>
@@ -2751,13 +2825,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142267904"/>
+        <c:crossAx val="326302720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="91"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142267904"/>
+        <c:axId val="326302720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2787,12 +2861,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142266368"/>
+        <c:crossAx val="326301184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142269824"/>
+        <c:axId val="33817728"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="25"/>
@@ -2827,12 +2901,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141755904"/>
+        <c:crossAx val="33819648"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141755904"/>
+        <c:axId val="33819648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2842,7 +2916,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142269824"/>
+        <c:crossAx val="33817728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2862,7 +2936,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2894,7 +2968,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2959,8 +3032,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141795328"/>
-        <c:axId val="141796864"/>
+        <c:axId val="162022912"/>
+        <c:axId val="162024448"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3013,11 +3086,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141805056"/>
-        <c:axId val="141798784"/>
+        <c:axId val="162036736"/>
+        <c:axId val="162034816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141795328"/>
+        <c:axId val="162022912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42735"/>
@@ -3029,13 +3102,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141796864"/>
+        <c:crossAx val="162024448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="91"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141796864"/>
+        <c:axId val="162024448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3063,19 +3136,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141795328"/>
+        <c:crossAx val="162022912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141798784"/>
+        <c:axId val="162034816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -3104,19 +3176,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141805056"/>
+        <c:crossAx val="162036736"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="141805056"/>
+        <c:axId val="162036736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3126,14 +3197,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141798784"/>
+        <c:crossAx val="162034816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3146,7 +3216,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3225,11 +3295,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="141834112"/>
-        <c:axId val="141835648"/>
+        <c:axId val="162049408"/>
+        <c:axId val="162063488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141834112"/>
+        <c:axId val="162049408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3239,7 +3309,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141835648"/>
+        <c:crossAx val="162063488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3247,7 +3317,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141835648"/>
+        <c:axId val="162063488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3276,7 +3346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141834112"/>
+        <c:crossAx val="162049408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3351,7 +3421,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="98" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3519,7 +3589,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9281160" cy="6012180"/>
+    <xdr:ext cx="9291735" cy="6002694"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagramm 1"/>
@@ -4204,13 +4274,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4218,10 +4288,13 @@
     <col min="1" max="1" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="11.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4249,8 +4322,17 @@
       <c r="I1" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -4278,8 +4360,17 @@
       <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>

</xml_diff>